<commit_message>
Added some info on Volatility + added all 504 lab exercises into the study-log-template.xlsx spreadsheet.
</commit_message>
<xml_diff>
--- a/study-log-template.xlsx
+++ b/study-log-template.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Dropbox\Education\College\Sans Institute of Technology\GSE\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Dropbox\Education\College\Sans Institute of Technology\GSE\GSE-Study\gse-study\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19920" windowHeight="10410" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19920" windowHeight="10410" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
     <sheet name="503 Lab Practice" sheetId="2" r:id="rId2"/>
+    <sheet name="504 Lab Practice" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="187" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="203">
   <si>
     <t>Date</t>
   </si>
@@ -388,13 +389,259 @@
   </si>
   <si>
     <t>How did you do?2</t>
+  </si>
+  <si>
+    <t>Windows Cheat Cheat</t>
+  </si>
+  <si>
+    <t>Launching cmd.exe</t>
+  </si>
+  <si>
+    <t>Network Usage - Netstat</t>
+  </si>
+  <si>
+    <t>Unusual Processes</t>
+  </si>
+  <si>
+    <t>Unusual Services</t>
+  </si>
+  <si>
+    <t>Unusual Registry Keys</t>
+  </si>
+  <si>
+    <t>Unusual Scheduled Tasks</t>
+  </si>
+  <si>
+    <t>Unusual Accounts</t>
+  </si>
+  <si>
+    <t>Enterprise-wide Indentification</t>
+  </si>
+  <si>
+    <t>Friday_Exchange.log</t>
+  </si>
+  <si>
+    <t>Friday.mans</t>
+  </si>
+  <si>
+    <t>Friday_SoftwareInventory.txt</t>
+  </si>
+  <si>
+    <t>Analyzing the Evil Insider</t>
+  </si>
+  <si>
+    <t>Checking Logins</t>
+  </si>
+  <si>
+    <t>Checking File Access</t>
+  </si>
+  <si>
+    <t>Checking Drives</t>
+  </si>
+  <si>
+    <t>InSSIDer</t>
+  </si>
+  <si>
+    <t>Finding Access Points</t>
+  </si>
+  <si>
+    <t>Nmap</t>
+  </si>
+  <si>
+    <t>Scanning Basics</t>
+  </si>
+  <si>
+    <t>Nessus</t>
+  </si>
+  <si>
+    <t>Starting Nessus</t>
+  </si>
+  <si>
+    <t>Setting and Starting a Scan</t>
+  </si>
+  <si>
+    <t>Reviewing Results</t>
+  </si>
+  <si>
+    <t>SMB Sessions</t>
+  </si>
+  <si>
+    <t>Starting SMB Session</t>
+  </si>
+  <si>
+    <t>Looking at Inbound and Outbound SMB Sessions</t>
+  </si>
+  <si>
+    <t>smbclient</t>
+  </si>
+  <si>
+    <t>rpcclient</t>
+  </si>
+  <si>
+    <t>nc.exe</t>
+  </si>
+  <si>
+    <t>netcat Lab 0</t>
+  </si>
+  <si>
+    <t>netcat Lab 1</t>
+  </si>
+  <si>
+    <t>netcat Lab 2</t>
+  </si>
+  <si>
+    <t>netcat Lab 3</t>
+  </si>
+  <si>
+    <t>netcat Lab 4</t>
+  </si>
+  <si>
+    <t>netcat Lab 5</t>
+  </si>
+  <si>
+    <t>ARP and MAC</t>
+  </si>
+  <si>
+    <t>Alice's ARP Cache</t>
+  </si>
+  <si>
+    <t>Router's ARP Cache</t>
+  </si>
+  <si>
+    <t>Analyzing Switch CAM Table</t>
+  </si>
+  <si>
+    <t>Searching DHCP Log</t>
+  </si>
+  <si>
+    <t>Metasploit Attack &amp; Analysis</t>
+  </si>
+  <si>
+    <t>Launching msfconsole and Viewing Exploits</t>
+  </si>
+  <si>
+    <t>Searching for Exploits</t>
+  </si>
+  <si>
+    <t>Configuring Metasploit to Use psexec</t>
+  </si>
+  <si>
+    <t>Configure Variables</t>
+  </si>
+  <si>
+    <t>Looking at Session Management</t>
+  </si>
+  <si>
+    <t>Analzying the Attack from Windows</t>
+  </si>
+  <si>
+    <t>John the Ripper</t>
+  </si>
+  <si>
+    <t>Creating Passwords to Crack</t>
+  </si>
+  <si>
+    <t>Retrieve Passwords on Linux</t>
+  </si>
+  <si>
+    <t>Running John the Ripper</t>
+  </si>
+  <si>
+    <t>Running John on Windows</t>
+  </si>
+  <si>
+    <t>XSS and SQLi</t>
+  </si>
+  <si>
+    <t>Starting the Server</t>
+  </si>
+  <si>
+    <t>Finding the XSS Vulnerability</t>
+  </si>
+  <si>
+    <t>Exploiting XSS</t>
+  </si>
+  <si>
+    <t>Using the Cookie</t>
+  </si>
+  <si>
+    <t>SQL Injection</t>
+  </si>
+  <si>
+    <t>Confirming SQL Injection</t>
+  </si>
+  <si>
+    <t>Pulling Records</t>
+  </si>
+  <si>
+    <t>Getting Hashes</t>
+  </si>
+  <si>
+    <t>Memory Analysis of Windows Attack</t>
+  </si>
+  <si>
+    <t>Invoking Volatility</t>
+  </si>
+  <si>
+    <t>Identify Processes by Connetion</t>
+  </si>
+  <si>
+    <t>Determine Command Line Invocations</t>
+  </si>
+  <si>
+    <t>The Missing Link</t>
+  </si>
+  <si>
+    <t>Netcat Activity</t>
+  </si>
+  <si>
+    <t>What is hot_pics.exe?</t>
+  </si>
+  <si>
+    <t>Shell History Analysis</t>
+  </si>
+  <si>
+    <t>Initial Action on System</t>
+  </si>
+  <si>
+    <t>File System Interactions</t>
+  </si>
+  <si>
+    <t>Launching Processes</t>
+  </si>
+  <si>
+    <t>Alternate Data Streams</t>
+  </si>
+  <si>
+    <t>Looking for Alternate Data Streams</t>
+  </si>
+  <si>
+    <t>Execitables in Alternate Data Streams</t>
+  </si>
+  <si>
+    <t>Using LADS</t>
+  </si>
+  <si>
+    <t>Covert Channels</t>
+  </si>
+  <si>
+    <t>Covert_TCP Receiver</t>
+  </si>
+  <si>
+    <t>Covert_TCP Sender</t>
+  </si>
+  <si>
+    <t>Plain Sight Convert Channels</t>
+  </si>
+  <si>
+    <t>VS Agent</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,16 +649,28 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -419,11 +678,31 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -434,11 +713,48 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="13">
+  <dxfs count="19">
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
@@ -474,10 +790,13 @@
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
@@ -494,33 +813,49 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0" headerRowDxfId="6" dataDxfId="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:E7" totalsRowShown="0" headerRowDxfId="18" dataDxfId="17">
   <autoFilter ref="A1:E7"/>
   <tableColumns count="5">
-    <tableColumn id="1" name="Date" dataDxfId="12"/>
-    <tableColumn id="2" name="Core Class" dataDxfId="11"/>
-    <tableColumn id="3" name="Subject" dataDxfId="10"/>
-    <tableColumn id="4" name="Practice" dataDxfId="9"/>
-    <tableColumn id="5" name="Time (hours)" dataDxfId="8"/>
+    <tableColumn id="1" name="Date" dataDxfId="16"/>
+    <tableColumn id="2" name="Core Class" dataDxfId="15"/>
+    <tableColumn id="3" name="Subject" dataDxfId="14"/>
+    <tableColumn id="4" name="Practice" dataDxfId="13"/>
+    <tableColumn id="5" name="Time (hours)" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J87" totalsRowShown="0" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A1:J87" totalsRowShown="0" headerRowDxfId="11">
   <autoFilter ref="A1:J87"/>
   <tableColumns count="10">
     <tableColumn id="1" name="Date Completed"/>
-    <tableColumn id="2" name="Core Class" dataDxfId="5"/>
-    <tableColumn id="3" name="Book #" dataDxfId="4"/>
-    <tableColumn id="4" name="Exercise Section" dataDxfId="3"/>
-    <tableColumn id="5" name="Exercise #" dataDxfId="2"/>
-    <tableColumn id="6" name="Exercise Topic" dataDxfId="1"/>
+    <tableColumn id="2" name="Core Class" dataDxfId="10"/>
+    <tableColumn id="3" name="Book #" dataDxfId="9"/>
+    <tableColumn id="4" name="Exercise Section" dataDxfId="8"/>
+    <tableColumn id="5" name="Exercise #" dataDxfId="7"/>
+    <tableColumn id="6" name="Exercise Topic" dataDxfId="6"/>
     <tableColumn id="7" name="Approach # 1"/>
     <tableColumn id="8" name="How did you do?"/>
     <tableColumn id="9" name="Approch # 2"/>
     <tableColumn id="10" name="How did you do?2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table24" displayName="Table24" ref="A1:G87" totalsRowShown="0" headerRowDxfId="5">
+  <autoFilter ref="A1:G87"/>
+  <tableColumns count="7">
+    <tableColumn id="1" name="Date Completed"/>
+    <tableColumn id="2" name="Core Class" dataDxfId="4"/>
+    <tableColumn id="3" name="Book #" dataDxfId="3"/>
+    <tableColumn id="4" name="Exercise Section" dataDxfId="2"/>
+    <tableColumn id="5" name="Exercise #" dataDxfId="1"/>
+    <tableColumn id="6" name="Exercise Topic" dataDxfId="0"/>
+    <tableColumn id="8" name="How did you do?"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -851,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J87"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2478,4 +2813,1380 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G87"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="3" width="15.5703125" customWidth="1"/>
+    <col min="4" max="4" width="33.85546875" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" customWidth="1"/>
+    <col min="6" max="6" width="36.7109375" customWidth="1"/>
+    <col min="7" max="7" width="22.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
+      <c r="B2" s="4">
+        <v>504</v>
+      </c>
+      <c r="C2" s="4">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="4">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
+      <c r="B3" s="4">
+        <v>504</v>
+      </c>
+      <c r="C3" s="5">
+        <v>1</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E3" s="5">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" s="4">
+        <v>504</v>
+      </c>
+      <c r="C4" s="4">
+        <v>1</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E4" s="4">
+        <v>3</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
+      <c r="B5" s="4">
+        <v>504</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E5" s="5">
+        <v>4</v>
+      </c>
+      <c r="F5" s="5" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1"/>
+      <c r="B6" s="4">
+        <v>504</v>
+      </c>
+      <c r="C6" s="4">
+        <v>1</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E6" s="4">
+        <v>5</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1"/>
+      <c r="B7" s="4">
+        <v>504</v>
+      </c>
+      <c r="C7" s="5">
+        <v>1</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E7" s="5">
+        <v>6</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="1"/>
+      <c r="B8" s="6">
+        <v>504</v>
+      </c>
+      <c r="C8" s="9">
+        <v>1</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>121</v>
+      </c>
+      <c r="E8" s="6">
+        <v>7</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="1"/>
+      <c r="B9" s="6">
+        <v>504</v>
+      </c>
+      <c r="C9" s="9">
+        <v>1</v>
+      </c>
+      <c r="D9" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="4">
+        <v>1</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="1"/>
+      <c r="B10" s="6">
+        <v>504</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E10" s="4">
+        <v>2</v>
+      </c>
+      <c r="F10" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1"/>
+      <c r="B11" s="6">
+        <v>504</v>
+      </c>
+      <c r="C11" s="9">
+        <v>1</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>129</v>
+      </c>
+      <c r="E11" s="4">
+        <v>3</v>
+      </c>
+      <c r="F11" s="4" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="1"/>
+      <c r="B12" s="6">
+        <v>504</v>
+      </c>
+      <c r="C12" s="9">
+        <v>1</v>
+      </c>
+      <c r="D12" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E12" s="4">
+        <v>1</v>
+      </c>
+      <c r="F12" s="4" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="1"/>
+      <c r="B13" s="6">
+        <v>504</v>
+      </c>
+      <c r="C13" s="9">
+        <v>1</v>
+      </c>
+      <c r="D13" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E13" s="4">
+        <v>2</v>
+      </c>
+      <c r="F13" s="4" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="6">
+        <v>504</v>
+      </c>
+      <c r="C14" s="9">
+        <v>1</v>
+      </c>
+      <c r="D14" s="6" t="s">
+        <v>133</v>
+      </c>
+      <c r="E14" s="4">
+        <v>3</v>
+      </c>
+      <c r="F14" s="4" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="1"/>
+      <c r="B15" s="6">
+        <v>504</v>
+      </c>
+      <c r="C15" s="9">
+        <v>2</v>
+      </c>
+      <c r="D15" s="6" t="s">
+        <v>137</v>
+      </c>
+      <c r="E15" s="4">
+        <v>1</v>
+      </c>
+      <c r="F15" s="4" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="1"/>
+      <c r="B16" s="6">
+        <v>504</v>
+      </c>
+      <c r="C16" s="9">
+        <v>2</v>
+      </c>
+      <c r="D16" s="4" t="s">
+        <v>139</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1</v>
+      </c>
+      <c r="F16" s="4" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A17" s="1"/>
+      <c r="B17" s="6">
+        <v>504</v>
+      </c>
+      <c r="C17" s="9">
+        <v>2</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E17" s="4">
+        <v>1</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="1"/>
+      <c r="B18" s="6">
+        <v>504</v>
+      </c>
+      <c r="C18" s="9">
+        <v>2</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E18" s="4">
+        <v>2</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="1"/>
+      <c r="B19" s="6">
+        <v>504</v>
+      </c>
+      <c r="C19" s="9">
+        <v>2</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>141</v>
+      </c>
+      <c r="E19" s="4">
+        <v>3</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A20" s="1"/>
+      <c r="B20" s="6">
+        <v>504</v>
+      </c>
+      <c r="C20" s="9">
+        <v>2</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E20" s="4">
+        <v>1</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A21" s="1"/>
+      <c r="B21" s="6">
+        <v>504</v>
+      </c>
+      <c r="C21" s="9">
+        <v>2</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E21" s="4">
+        <v>2</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A22" s="1"/>
+      <c r="B22" s="6">
+        <v>504</v>
+      </c>
+      <c r="C22" s="9">
+        <v>2</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E22" s="4">
+        <v>3</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A23" s="1"/>
+      <c r="B23" s="6">
+        <v>504</v>
+      </c>
+      <c r="C23" s="9">
+        <v>2</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>145</v>
+      </c>
+      <c r="E23" s="4">
+        <v>4</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A24" s="1"/>
+      <c r="B24" s="6">
+        <v>504</v>
+      </c>
+      <c r="C24" s="9">
+        <v>3</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E24" s="4">
+        <v>1</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="6">
+        <v>504</v>
+      </c>
+      <c r="C25" s="9">
+        <v>3</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E25" s="4">
+        <v>2</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A26" s="1"/>
+      <c r="B26" s="6">
+        <v>504</v>
+      </c>
+      <c r="C26" s="9">
+        <v>3</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E26" s="4">
+        <v>3</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A27" s="1"/>
+      <c r="B27" s="6">
+        <v>504</v>
+      </c>
+      <c r="C27" s="9">
+        <v>3</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E27" s="4">
+        <v>4</v>
+      </c>
+      <c r="F27" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A28" s="1"/>
+      <c r="B28" s="6">
+        <v>504</v>
+      </c>
+      <c r="C28" s="9">
+        <v>3</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E28" s="4">
+        <v>4</v>
+      </c>
+      <c r="F28" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A29" s="1"/>
+      <c r="B29" s="6">
+        <v>504</v>
+      </c>
+      <c r="C29" s="9">
+        <v>3</v>
+      </c>
+      <c r="D29" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="E29" s="4">
+        <v>4</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A30" s="1"/>
+      <c r="B30" s="4">
+        <v>504</v>
+      </c>
+      <c r="C30" s="5">
+        <v>3</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E30" s="4">
+        <v>1</v>
+      </c>
+      <c r="F30" s="4" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A31" s="1"/>
+      <c r="B31" s="4">
+        <v>504</v>
+      </c>
+      <c r="C31" s="5">
+        <v>3</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E31" s="4">
+        <v>2</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A32" s="1"/>
+      <c r="B32" s="4">
+        <v>504</v>
+      </c>
+      <c r="C32" s="5">
+        <v>3</v>
+      </c>
+      <c r="D32" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E32" s="4">
+        <v>3</v>
+      </c>
+      <c r="F32" s="4" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="1"/>
+      <c r="B33" s="4">
+        <v>504</v>
+      </c>
+      <c r="C33" s="5">
+        <v>3</v>
+      </c>
+      <c r="D33" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="E33" s="4">
+        <v>4</v>
+      </c>
+      <c r="F33" s="4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A34" s="1"/>
+      <c r="B34" s="4">
+        <v>504</v>
+      </c>
+      <c r="C34" s="5">
+        <v>3</v>
+      </c>
+      <c r="D34" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E34" s="4">
+        <v>1</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A35" s="1"/>
+      <c r="B35" s="4">
+        <v>504</v>
+      </c>
+      <c r="C35" s="5">
+        <v>3</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E35" s="4">
+        <v>2</v>
+      </c>
+      <c r="F35" s="4" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A36" s="1"/>
+      <c r="B36" s="4">
+        <v>504</v>
+      </c>
+      <c r="C36" s="5">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E36" s="4">
+        <v>3</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A37" s="1"/>
+      <c r="B37" s="4">
+        <v>504</v>
+      </c>
+      <c r="C37" s="5">
+        <v>3</v>
+      </c>
+      <c r="D37" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E37" s="6">
+        <v>4</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A38" s="1"/>
+      <c r="B38" s="4">
+        <v>504</v>
+      </c>
+      <c r="C38" s="5">
+        <v>3</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E38" s="7">
+        <v>5</v>
+      </c>
+      <c r="F38" s="7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A39" s="1"/>
+      <c r="B39" s="4">
+        <v>504</v>
+      </c>
+      <c r="C39" s="5">
+        <v>3</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="E39" s="7">
+        <v>6</v>
+      </c>
+      <c r="F39" s="7" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" s="4">
+        <v>504</v>
+      </c>
+      <c r="C40" s="5">
+        <v>4</v>
+      </c>
+      <c r="D40" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E40" s="7">
+        <v>1</v>
+      </c>
+      <c r="F40" s="7" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" s="4">
+        <v>504</v>
+      </c>
+      <c r="C41" s="5">
+        <v>4</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E41" s="7">
+        <v>2</v>
+      </c>
+      <c r="F41" s="7" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A42" s="1"/>
+      <c r="B42" s="4">
+        <v>504</v>
+      </c>
+      <c r="C42" s="5">
+        <v>4</v>
+      </c>
+      <c r="D42" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E42" s="7">
+        <v>3</v>
+      </c>
+      <c r="F42" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A43" s="1"/>
+      <c r="B43" s="4">
+        <v>504</v>
+      </c>
+      <c r="C43" s="5">
+        <v>4</v>
+      </c>
+      <c r="D43" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E43" s="7">
+        <v>4</v>
+      </c>
+      <c r="F43" s="7" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A44" s="1"/>
+      <c r="B44" s="4">
+        <v>504</v>
+      </c>
+      <c r="C44" s="5">
+        <v>4</v>
+      </c>
+      <c r="D44" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E44" s="8">
+        <v>1</v>
+      </c>
+      <c r="F44" s="8" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A45" s="1"/>
+      <c r="B45" s="4">
+        <v>504</v>
+      </c>
+      <c r="C45" s="5">
+        <v>4</v>
+      </c>
+      <c r="D45" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E45" s="7">
+        <v>2</v>
+      </c>
+      <c r="F45" s="7" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A46" s="1"/>
+      <c r="B46" s="4">
+        <v>504</v>
+      </c>
+      <c r="C46" s="5">
+        <v>4</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E46" s="7">
+        <v>3</v>
+      </c>
+      <c r="F46" s="7" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A47" s="1"/>
+      <c r="B47" s="4">
+        <v>504</v>
+      </c>
+      <c r="C47" s="5">
+        <v>4</v>
+      </c>
+      <c r="D47" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E47" s="7">
+        <v>4</v>
+      </c>
+      <c r="F47" s="7" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A48" s="1"/>
+      <c r="B48" s="4">
+        <v>504</v>
+      </c>
+      <c r="C48" s="5">
+        <v>4</v>
+      </c>
+      <c r="D48" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E48" s="7">
+        <v>5</v>
+      </c>
+      <c r="F48" s="7" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A49" s="1"/>
+      <c r="B49" s="4">
+        <v>504</v>
+      </c>
+      <c r="C49" s="5">
+        <v>4</v>
+      </c>
+      <c r="D49" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E49" s="7">
+        <v>6</v>
+      </c>
+      <c r="F49" s="7" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A50" s="1"/>
+      <c r="B50" s="4">
+        <v>504</v>
+      </c>
+      <c r="C50" s="5">
+        <v>4</v>
+      </c>
+      <c r="D50" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E50" s="7">
+        <v>7</v>
+      </c>
+      <c r="F50" s="7" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A51" s="2"/>
+      <c r="B51" s="4">
+        <v>504</v>
+      </c>
+      <c r="C51" s="5">
+        <v>4</v>
+      </c>
+      <c r="D51" s="8" t="s">
+        <v>174</v>
+      </c>
+      <c r="E51" s="7">
+        <v>8</v>
+      </c>
+      <c r="F51" s="7" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A52" s="2"/>
+      <c r="B52" s="7">
+        <v>504</v>
+      </c>
+      <c r="C52" s="10">
+        <v>5</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E52" s="7">
+        <v>1</v>
+      </c>
+      <c r="F52" s="7" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A53" s="2"/>
+      <c r="B53" s="7">
+        <v>504</v>
+      </c>
+      <c r="C53" s="10">
+        <v>5</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E53" s="8">
+        <v>2</v>
+      </c>
+      <c r="F53" s="8" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A54" s="2"/>
+      <c r="B54" s="7">
+        <v>504</v>
+      </c>
+      <c r="C54" s="10">
+        <v>5</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E54" s="7">
+        <v>3</v>
+      </c>
+      <c r="F54" s="7" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A55" s="2"/>
+      <c r="B55" s="7">
+        <v>504</v>
+      </c>
+      <c r="C55" s="10">
+        <v>5</v>
+      </c>
+      <c r="D55" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E55" s="7">
+        <v>4</v>
+      </c>
+      <c r="F55" s="7" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A56" s="2"/>
+      <c r="B56" s="7">
+        <v>504</v>
+      </c>
+      <c r="C56" s="10">
+        <v>5</v>
+      </c>
+      <c r="D56" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E56" s="7">
+        <v>5</v>
+      </c>
+      <c r="F56" s="7" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="7">
+        <v>504</v>
+      </c>
+      <c r="C57" s="10">
+        <v>5</v>
+      </c>
+      <c r="D57" s="7" t="s">
+        <v>183</v>
+      </c>
+      <c r="E57" s="7">
+        <v>6</v>
+      </c>
+      <c r="F57" s="7" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="7">
+        <v>504</v>
+      </c>
+      <c r="C58" s="10">
+        <v>5</v>
+      </c>
+      <c r="D58" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="E58" s="7">
+        <v>1</v>
+      </c>
+      <c r="F58" s="7" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="7">
+        <v>504</v>
+      </c>
+      <c r="C59" s="10">
+        <v>5</v>
+      </c>
+      <c r="D59" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="E59" s="7">
+        <v>2</v>
+      </c>
+      <c r="F59" s="7" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="7">
+        <v>504</v>
+      </c>
+      <c r="C60" s="10">
+        <v>5</v>
+      </c>
+      <c r="D60" s="7" t="s">
+        <v>190</v>
+      </c>
+      <c r="E60" s="7">
+        <v>3</v>
+      </c>
+      <c r="F60" s="7" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="7">
+        <v>504</v>
+      </c>
+      <c r="C61" s="10">
+        <v>5</v>
+      </c>
+      <c r="D61" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E61" s="7">
+        <v>1</v>
+      </c>
+      <c r="F61" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="7">
+        <v>504</v>
+      </c>
+      <c r="C62" s="10">
+        <v>5</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E62" s="8">
+        <v>2</v>
+      </c>
+      <c r="F62" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B63" s="7">
+        <v>504</v>
+      </c>
+      <c r="C63" s="10">
+        <v>5</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E63" s="7">
+        <v>3</v>
+      </c>
+      <c r="F63" s="7" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="7">
+        <v>504</v>
+      </c>
+      <c r="C64" s="10">
+        <v>5</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>194</v>
+      </c>
+      <c r="E64" s="7">
+        <v>4</v>
+      </c>
+      <c r="F64" s="7" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B65" s="3">
+        <v>504</v>
+      </c>
+      <c r="C65" s="1">
+        <v>5</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E65" s="1">
+        <v>1</v>
+      </c>
+      <c r="F65" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B66" s="3">
+        <v>504</v>
+      </c>
+      <c r="C66" s="1">
+        <v>5</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E66" s="1">
+        <v>2</v>
+      </c>
+      <c r="F66" s="1" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B67" s="3">
+        <v>504</v>
+      </c>
+      <c r="C67" s="1">
+        <v>5</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E67" s="1">
+        <v>3</v>
+      </c>
+      <c r="F67" s="1" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B68" s="3">
+        <v>504</v>
+      </c>
+      <c r="C68" s="1">
+        <v>5</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="E68" s="1">
+        <v>4</v>
+      </c>
+      <c r="F68" s="1" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B69" s="3"/>
+      <c r="C69" s="1"/>
+      <c r="D69" s="1"/>
+      <c r="E69" s="1"/>
+      <c r="F69" s="1"/>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B70" s="3"/>
+      <c r="C70" s="1"/>
+      <c r="D70" s="1"/>
+      <c r="E70" s="1"/>
+      <c r="F70" s="1"/>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B71" s="3"/>
+      <c r="C71" s="1"/>
+      <c r="D71" s="1"/>
+      <c r="E71" s="1"/>
+      <c r="F71" s="1"/>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B72" s="3"/>
+      <c r="C72" s="1"/>
+      <c r="D72" s="1"/>
+      <c r="E72" s="1"/>
+      <c r="F72" s="1"/>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B73" s="3"/>
+      <c r="C73" s="1"/>
+      <c r="D73" s="1"/>
+      <c r="E73" s="1"/>
+      <c r="F73" s="1"/>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B74" s="3"/>
+      <c r="C74" s="1"/>
+      <c r="D74" s="1"/>
+      <c r="E74" s="1"/>
+      <c r="F74" s="1"/>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B75" s="3"/>
+      <c r="C75" s="1"/>
+      <c r="D75" s="1"/>
+      <c r="E75" s="1"/>
+      <c r="F75" s="1"/>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B76" s="3"/>
+      <c r="C76" s="1"/>
+      <c r="D76" s="1"/>
+      <c r="E76" s="1"/>
+      <c r="F76" s="1"/>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B77" s="3"/>
+      <c r="C77" s="1"/>
+      <c r="D77" s="1"/>
+      <c r="E77" s="1"/>
+      <c r="F77" s="1"/>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B78" s="3"/>
+      <c r="C78" s="1"/>
+      <c r="D78" s="1"/>
+      <c r="E78" s="1"/>
+      <c r="F78" s="1"/>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B79" s="3"/>
+      <c r="C79" s="1"/>
+      <c r="D79" s="1"/>
+      <c r="E79" s="1"/>
+      <c r="F79" s="1"/>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B80" s="3"/>
+      <c r="C80" s="1"/>
+      <c r="D80" s="1"/>
+      <c r="E80" s="1"/>
+      <c r="F80" s="1"/>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B81" s="3"/>
+      <c r="C81" s="1"/>
+      <c r="D81" s="1"/>
+      <c r="E81" s="1"/>
+      <c r="F81" s="1"/>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B82" s="3"/>
+      <c r="C82" s="1"/>
+      <c r="D82" s="1"/>
+      <c r="E82" s="1"/>
+      <c r="F82" s="1"/>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B83" s="3"/>
+      <c r="C83" s="1"/>
+      <c r="D83" s="1"/>
+      <c r="E83" s="1"/>
+      <c r="F83" s="1"/>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B84" s="3"/>
+      <c r="C84" s="1"/>
+      <c r="D84" s="1"/>
+      <c r="E84" s="1"/>
+      <c r="F84" s="1"/>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B85" s="3"/>
+      <c r="C85" s="1"/>
+      <c r="D85" s="1"/>
+      <c r="E85" s="1"/>
+      <c r="F85" s="1"/>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B86" s="3"/>
+      <c r="C86" s="1"/>
+      <c r="D86" s="1"/>
+      <c r="E86" s="1"/>
+      <c r="F86" s="1"/>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B87" s="3"/>
+      <c r="C87" s="1"/>
+      <c r="D87" s="1"/>
+      <c r="E87" s="1"/>
+      <c r="F87" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>